<commit_message>
Replace the 'isAggregated' column with 'type' for a more abstract implementation.
</commit_message>
<xml_diff>
--- a/tse-app/config/tablesSchema.xlsx
+++ b/tse-app/config/tablesSchema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thanos\Desktop\tse-efsa\tse-reporting-tool\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panos\Documents\Git\CRI\EFSA\tse-app\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695D54EE-AABF-41F7-93FC-478C6BC41B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C31BD4-B8C5-4B94-840F-60BD89B9E4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="26355" windowHeight="15600" tabRatio="690" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="690" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="489">
   <si>
     <t>Type</t>
   </si>
@@ -1495,9 +1495,6 @@
   </si>
   <si>
     <t>aggregatorId</t>
-  </si>
-  <si>
-    <t>isAggregated</t>
   </si>
   <si>
     <t>isAmended</t>
@@ -1642,7 +1639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1667,9 +1664,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3628,25 +3622,25 @@
       <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="14" width="14.140625" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.5859375" customWidth="1"/>
+    <col min="2" max="2" width="26.41015625" customWidth="1"/>
+    <col min="3" max="3" width="12.29296875" customWidth="1"/>
+    <col min="4" max="4" width="18.29296875" customWidth="1"/>
+    <col min="5" max="5" width="35.29296875" customWidth="1"/>
+    <col min="6" max="6" width="14.703125" customWidth="1"/>
+    <col min="7" max="7" width="23.87890625" customWidth="1"/>
+    <col min="8" max="8" width="14.1171875" customWidth="1"/>
+    <col min="9" max="9" width="15.87890625" customWidth="1"/>
+    <col min="10" max="10" width="12.5859375" customWidth="1"/>
+    <col min="11" max="11" width="12.703125" customWidth="1"/>
+    <col min="12" max="14" width="14.1171875" customWidth="1"/>
+    <col min="15" max="15" width="14.703125" customWidth="1"/>
+    <col min="16" max="16" width="14.1171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -3705,7 +3699,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>136</v>
       </c>
@@ -3738,7 +3732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>137</v>
       </c>
@@ -3771,7 +3765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -3823,24 +3817,24 @@
       <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.28515625" customWidth="1"/>
-    <col min="13" max="14" width="14.140625" customWidth="1"/>
-    <col min="15" max="16" width="14.7109375" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.87890625" customWidth="1"/>
+    <col min="3" max="3" width="9.41015625" customWidth="1"/>
+    <col min="4" max="4" width="20.703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.41015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.29296875" customWidth="1"/>
+    <col min="7" max="7" width="23.87890625" customWidth="1"/>
+    <col min="8" max="8" width="12.703125" customWidth="1"/>
+    <col min="9" max="9" width="10.5859375" customWidth="1"/>
+    <col min="11" max="11" width="12.87890625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.29296875" customWidth="1"/>
+    <col min="13" max="14" width="14.1171875" customWidth="1"/>
+    <col min="15" max="16" width="14.703125" customWidth="1"/>
+    <col min="17" max="17" width="14.1171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -3899,7 +3893,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>117</v>
       </c>
@@ -3934,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>413</v>
       </c>
@@ -3984,7 +3978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>120</v>
       </c>
@@ -4022,7 +4016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>122</v>
       </c>
@@ -4060,7 +4054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>124</v>
       </c>
@@ -4098,7 +4092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>475</v>
       </c>
@@ -4136,7 +4130,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>126</v>
       </c>
@@ -4174,7 +4168,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>129</v>
       </c>
@@ -4212,7 +4206,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>132</v>
       </c>
@@ -4250,7 +4244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>476</v>
       </c>
@@ -4288,7 +4282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>330</v>
       </c>
@@ -4327,7 +4321,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>328</v>
       </c>
@@ -4366,7 +4360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>329</v>
       </c>
@@ -4405,7 +4399,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A15" s="5" t="s">
         <v>479</v>
       </c>
@@ -4460,31 +4454,31 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="62.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="33.42578125" customWidth="1"/>
-    <col min="14" max="14" width="38.85546875" customWidth="1"/>
-    <col min="15" max="15" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.5859375" customWidth="1"/>
+    <col min="3" max="3" width="10.703125" customWidth="1"/>
+    <col min="4" max="4" width="18.29296875" customWidth="1"/>
+    <col min="5" max="5" width="62.29296875" customWidth="1"/>
+    <col min="6" max="6" width="13.5859375" customWidth="1"/>
+    <col min="7" max="7" width="23.87890625" customWidth="1"/>
+    <col min="8" max="8" width="14.1171875" customWidth="1"/>
+    <col min="9" max="9" width="10.5859375" customWidth="1"/>
+    <col min="10" max="10" width="10.29296875" customWidth="1"/>
+    <col min="11" max="11" width="14.41015625" customWidth="1"/>
+    <col min="12" max="12" width="14.1171875" customWidth="1"/>
+    <col min="13" max="13" width="33.41015625" customWidth="1"/>
+    <col min="14" max="14" width="38.87890625" customWidth="1"/>
+    <col min="15" max="15" width="35.29296875" customWidth="1"/>
     <col min="16" max="16" width="22" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.1171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -4543,7 +4537,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>166</v>
       </c>
@@ -4591,7 +4585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>167</v>
       </c>
@@ -4639,7 +4633,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>183</v>
       </c>
@@ -4677,7 +4671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
         <v>117</v>
       </c>
@@ -4724,7 +4718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>177</v>
       </c>
@@ -4747,7 +4741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>315</v>
       </c>
@@ -4777,7 +4771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>239</v>
       </c>
@@ -4808,7 +4802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>386</v>
       </c>
@@ -4836,7 +4830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>387</v>
       </c>
@@ -4864,7 +4858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>245</v>
       </c>
@@ -4900,7 +4894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>240</v>
       </c>
@@ -4936,7 +4930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>368</v>
       </c>
@@ -4967,12 +4961,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>488</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>488</v>
+        <v>96</v>
       </c>
       <c r="D14" s="6"/>
       <c r="F14" t="s">
@@ -4995,7 +4989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>487</v>
       </c>
@@ -5023,38 +5017,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
         <v>244</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" t="s">
         <v>244</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22" t="s">
+      <c r="D16" s="6"/>
+      <c r="F16" t="s">
         <v>174</v>
       </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="24"/>
-      <c r="O16" s="22"/>
-      <c r="Q16" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22" t="s">
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M16" s="10"/>
+      <c r="Q16" t="s">
+        <v>5</v>
+      </c>
+      <c r="S16" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5078,28 +5065,28 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.41015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5859375" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="68.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="74.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="78.42578125" customWidth="1"/>
-    <col min="14" max="14" width="45.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.41015625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="68.29296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.29296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="74.703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="78.41015625" customWidth="1"/>
+    <col min="14" max="14" width="45.1171875" customWidth="1"/>
     <col min="15" max="15" width="52" customWidth="1"/>
-    <col min="16" max="16" width="71.28515625" customWidth="1"/>
+    <col min="16" max="16" width="71.29296875" customWidth="1"/>
     <col min="17" max="17" width="20" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -5158,7 +5145,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -5199,7 +5186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -5249,7 +5236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -5296,7 +5283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -5340,7 +5327,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -5384,7 +5371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>379</v>
       </c>
@@ -5431,7 +5418,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -5484,7 +5471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -5537,7 +5524,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -5587,7 +5574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" s="12" t="s">
         <v>392</v>
       </c>
@@ -5619,7 +5606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -5657,7 +5644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -5695,7 +5682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -5733,7 +5720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -5774,7 +5761,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -5812,7 +5799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -5850,7 +5837,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>265</v>
       </c>
@@ -5891,7 +5878,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>262</v>
       </c>
@@ -5932,7 +5919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -5964,7 +5951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -5996,7 +5983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>343</v>
       </c>
@@ -6022,7 +6009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -6054,7 +6041,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -6089,7 +6076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>177</v>
       </c>
@@ -6109,7 +6096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -6141,7 +6128,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -6170,7 +6157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -6205,7 +6192,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>172</v>
       </c>
@@ -6225,7 +6212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -6260,7 +6247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -6292,7 +6279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -6324,7 +6311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -6359,7 +6346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -6388,7 +6375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -6420,7 +6407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>399</v>
       </c>
@@ -6449,7 +6436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -6484,7 +6471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -6516,7 +6503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -6551,7 +6538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>222</v>
       </c>
@@ -6577,7 +6564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -6612,7 +6599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>178</v>
       </c>
@@ -6632,12 +6619,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B43" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F43" t="s">
         <v>174</v>
@@ -6675,27 +6662,27 @@
       <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.85546875" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.41015625" customWidth="1"/>
+    <col min="3" max="3" width="14.41015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.87890625" customWidth="1"/>
+    <col min="5" max="5" width="56.703125" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="143.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="82.85546875" customWidth="1"/>
-    <col min="10" max="10" width="52.140625" customWidth="1"/>
-    <col min="11" max="11" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.140625" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" customWidth="1"/>
-    <col min="14" max="14" width="38.7109375" customWidth="1"/>
-    <col min="15" max="16" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23.87890625" customWidth="1"/>
+    <col min="8" max="8" width="143.1171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="82.87890625" customWidth="1"/>
+    <col min="10" max="10" width="52.1171875" customWidth="1"/>
+    <col min="11" max="11" width="29.29296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46.1171875" customWidth="1"/>
+    <col min="13" max="13" width="29.703125" customWidth="1"/>
+    <col min="14" max="14" width="38.703125" customWidth="1"/>
+    <col min="15" max="16" width="22.87890625" customWidth="1"/>
     <col min="17" max="17" width="20" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" customWidth="1"/>
+    <col min="19" max="19" width="10.1171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -6754,7 +6741,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>410</v>
       </c>
@@ -6795,7 +6782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -6830,7 +6817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -6880,7 +6867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>379</v>
       </c>
@@ -6924,7 +6911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -6965,7 +6952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>190</v>
       </c>
@@ -7003,7 +6990,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>201</v>
       </c>
@@ -7039,7 +7026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>205</v>
       </c>
@@ -7074,7 +7061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -7109,7 +7096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -7144,7 +7131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>213</v>
       </c>
@@ -7185,7 +7172,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>194</v>
       </c>
@@ -7228,7 +7215,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>208</v>
       </c>
@@ -7266,7 +7253,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>278</v>
       </c>
@@ -7304,7 +7291,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>282</v>
       </c>
@@ -7339,7 +7326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>277</v>
       </c>
@@ -7380,7 +7367,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>287</v>
       </c>
@@ -7415,7 +7402,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>290</v>
       </c>
@@ -7450,7 +7437,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>220</v>
       </c>
@@ -7470,7 +7457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>172</v>
       </c>
@@ -7490,7 +7477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>343</v>
       </c>
@@ -7536,26 +7523,26 @@
       <selection pane="bottomRight" activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" customWidth="1"/>
-    <col min="5" max="5" width="43.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.29296875" customWidth="1"/>
+    <col min="3" max="3" width="25.5859375" customWidth="1"/>
+    <col min="4" max="4" width="32.29296875" customWidth="1"/>
+    <col min="5" max="5" width="43.1171875" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" customWidth="1"/>
-    <col min="9" max="9" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.87890625" customWidth="1"/>
+    <col min="8" max="8" width="49.41015625" customWidth="1"/>
+    <col min="9" max="9" width="51.29296875" customWidth="1"/>
     <col min="10" max="10" width="55" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="67.140625" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="50.7109375" customWidth="1"/>
+    <col min="12" max="12" width="67.1171875" customWidth="1"/>
+    <col min="13" max="13" width="19.1171875" customWidth="1"/>
+    <col min="14" max="14" width="50.703125" customWidth="1"/>
     <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="102.85546875" customWidth="1"/>
+    <col min="16" max="16" width="102.87890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -7611,7 +7598,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>265</v>
       </c>
@@ -7649,7 +7636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>262</v>
       </c>
@@ -7687,7 +7674,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -7734,7 +7721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -7760,7 +7747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -7804,7 +7791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -7842,7 +7829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -7886,7 +7873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>406</v>
       </c>
@@ -7924,7 +7911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>226</v>
       </c>
@@ -7944,7 +7931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>225</v>
       </c>
@@ -7973,7 +7960,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>401</v>
       </c>
@@ -7999,7 +7986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -8034,7 +8021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>319</v>
       </c>
@@ -8057,7 +8044,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -8092,7 +8079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -8124,7 +8111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>375</v>
       </c>
@@ -8150,7 +8137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -8182,7 +8169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -8220,7 +8207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -8252,7 +8239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>172</v>
       </c>
@@ -8272,7 +8259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -8304,7 +8291,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -8345,7 +8332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>253</v>
       </c>
@@ -8377,7 +8364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>250</v>
       </c>
@@ -8406,7 +8393,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -8438,7 +8425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>213</v>
       </c>
@@ -8470,7 +8457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -8502,7 +8489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>271</v>
       </c>
@@ -8537,7 +8524,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -8569,7 +8556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -8598,7 +8585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -8636,7 +8623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>399</v>
       </c>
@@ -8665,7 +8652,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -8697,7 +8684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -8729,7 +8716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>268</v>
       </c>
@@ -8758,7 +8745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -8793,7 +8780,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>222</v>
       </c>
@@ -8825,7 +8812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>402</v>
       </c>
@@ -8860,7 +8847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -8895,7 +8882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>379</v>
       </c>
@@ -8921,7 +8908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>220</v>
       </c>
@@ -8941,7 +8928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>338</v>
       </c>
@@ -8992,14 +8979,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.29296875" customWidth="1"/>
+    <col min="2" max="2" width="39.29296875" customWidth="1"/>
+    <col min="3" max="3" width="18.5859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>168</v>
       </c>
@@ -9010,7 +8997,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -9021,7 +9008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>171</v>
       </c>
@@ -9032,7 +9019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>176</v>
       </c>
@@ -9043,7 +9030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>176</v>
       </c>
@@ -9054,7 +9041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -9065,7 +9052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>175</v>
       </c>
@@ -9076,7 +9063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>221</v>
       </c>
@@ -9087,7 +9074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>170</v>
       </c>
@@ -9098,7 +9085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>171</v>
       </c>
@@ -9109,7 +9096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>170</v>
       </c>
@@ -9120,7 +9107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>175</v>
       </c>
@@ -9147,12 +9134,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>186</v>
       </c>
@@ -9160,7 +9147,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -9168,7 +9155,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>170</v>
       </c>
@@ -9176,7 +9163,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>175</v>
       </c>
@@ -9184,7 +9171,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>176</v>
       </c>
@@ -9192,7 +9179,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>221</v>
       </c>
@@ -9200,7 +9187,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>227</v>
       </c>
@@ -9227,30 +9214,30 @@
       <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="0.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" customWidth="1"/>
-    <col min="12" max="12" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="0.703125" customWidth="1"/>
+    <col min="3" max="3" width="13.703125" customWidth="1"/>
+    <col min="4" max="4" width="3.1171875" customWidth="1"/>
+    <col min="5" max="5" width="36.87890625" customWidth="1"/>
+    <col min="6" max="6" width="15.41015625" customWidth="1"/>
+    <col min="7" max="7" width="2.87890625" customWidth="1"/>
+    <col min="8" max="8" width="2.29296875" customWidth="1"/>
+    <col min="9" max="9" width="6.703125" customWidth="1"/>
+    <col min="10" max="10" width="4.41015625" customWidth="1"/>
+    <col min="11" max="11" width="4.1171875" customWidth="1"/>
+    <col min="12" max="12" width="3.29296875" customWidth="1"/>
     <col min="13" max="13" width="4" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" customWidth="1"/>
-    <col min="15" max="15" width="19.85546875" customWidth="1"/>
-    <col min="16" max="16" width="95.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.85546875" customWidth="1"/>
+    <col min="14" max="14" width="5.29296875" customWidth="1"/>
+    <col min="15" max="15" width="19.87890625" customWidth="1"/>
+    <col min="16" max="16" width="95.1171875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.87890625" customWidth="1"/>
     <col min="18" max="18" width="3" customWidth="1"/>
-    <col min="19" max="19" width="2.28515625" customWidth="1"/>
+    <col min="19" max="19" width="2.29296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -9309,7 +9296,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -9338,7 +9325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -9367,7 +9354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -9390,7 +9377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -9418,7 +9405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>233</v>
       </c>
@@ -9441,7 +9428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>242</v>
       </c>
@@ -9464,7 +9451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>244</v>
       </c>
@@ -9487,7 +9474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>304</v>
       </c>
@@ -9510,7 +9497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>235</v>
       </c>
@@ -9536,7 +9523,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -9559,7 +9546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>248</v>
       </c>
@@ -9582,7 +9569,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>340</v>
       </c>
@@ -9602,7 +9589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>312</v>
       </c>
@@ -9625,7 +9612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>172</v>
       </c>
@@ -9639,7 +9626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>178</v>
       </c>

</xml_diff>